<commit_message>
Renamed MTOM_EnsembleOutput and MTOM_24MS_Comparison files to include the month they were run
Added 10/50/90 comparison charts of for the september MTOM run
</commit_message>
<xml_diff>
--- a/RW Files/TestModelRuns/08_August Models/Comparison Charts_AUGtest.xlsx
+++ b/RW Files/TestModelRuns/08_August Models/Comparison Charts_AUGtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apivarnik\Desktop\GIT\MTOM\RW Files\TestModelRuns\08_August Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9BC7D6-E814-42F9-BC17-71DC5C5EA2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FBC56F-1777-4E86-85AF-589A7FDFEB5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B484995-6852-4B2C-A888-3922C388AA28}"/>
+    <workbookView xWindow="30180" yWindow="1860" windowWidth="27240" windowHeight="10485" activeTab="1" xr2:uid="{0B484995-6852-4B2C-A888-3922C388AA28}"/>
   </bookViews>
   <sheets>
     <sheet name="Mead Chart" sheetId="2" r:id="rId1"/>
@@ -3069,7 +3069,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Lake Powell End of Month Elevation - July 2020 MTOM</a:t>
+              <a:t>Lake Powell End of Month Elevation - August 2020 MTOM</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7038,7 +7038,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BBBA9ED6-B4C5-4DBF-9AE1-C7E8BD8300B1}">
   <sheetPr codeName="Chart1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="65" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7049,7 +7049,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{4B1FF22C-1021-4953-AABB-6BBC3FA86BAD}">
   <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7060,7 +7060,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6293304"/>
+    <xdr:ext cx="8673523" cy="6306705"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7093,7 +7093,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8673523" cy="6306705"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">

</xml_diff>